<commit_message>
Most of the work grouped as function
</commit_message>
<xml_diff>
--- a/AD-OCS/Working SULFUR/data/amoco_HN.xlsx
+++ b/AD-OCS/Working SULFUR/data/amoco_HN.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://polimi365-my.sharepoint.com/personal/10619235_polimi_it/Documents/Documenti/GitHub/AD-OCS/AD-OCS/Working SULFUR/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="68" documentId="8_{854BF156-97D4-495F-9740-E4B6A28AF2BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{49E0F200-CBBC-4AA5-80A9-7079D2C4ED51}"/>
+  <xr:revisionPtr revIDLastSave="93" documentId="8_{854BF156-97D4-495F-9740-E4B6A28AF2BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{251858C6-71C6-4171-89A6-1893065FDBAD}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="1" activeTab="2" xr2:uid="{937B5A09-45AC-4F43-9144-B848BCA4D579}"/>
   </bookViews>
@@ -2206,10 +2206,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{22C458D2-0390-4007-98A4-66EBEC10F814}">
-  <dimension ref="A1:F10"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="F5" sqref="A4:F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2251,12 +2251,12 @@
         <v>1</v>
       </c>
       <c r="F2">
-        <v>1</v>
+        <v>1.2</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3">
-        <v>25</v>
+        <v>120</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -2271,147 +2271,7 @@
         <v>1</v>
       </c>
       <c r="F3">
-        <v>1.2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A4">
-        <v>50</v>
-      </c>
-      <c r="B4">
         <v>1</v>
-      </c>
-      <c r="C4">
-        <v>1</v>
-      </c>
-      <c r="D4">
-        <v>1</v>
-      </c>
-      <c r="E4">
-        <v>1</v>
-      </c>
-      <c r="F4">
-        <v>1.1000000000000001</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A5">
-        <v>100</v>
-      </c>
-      <c r="B5">
-        <v>1</v>
-      </c>
-      <c r="C5">
-        <v>1</v>
-      </c>
-      <c r="D5">
-        <v>1</v>
-      </c>
-      <c r="E5">
-        <v>1</v>
-      </c>
-      <c r="F5">
-        <v>1.25</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A6">
-        <v>120</v>
-      </c>
-      <c r="B6">
-        <v>1</v>
-      </c>
-      <c r="C6">
-        <v>1</v>
-      </c>
-      <c r="D6">
-        <v>1</v>
-      </c>
-      <c r="E6">
-        <v>1</v>
-      </c>
-      <c r="F6">
-        <v>1.3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A7">
-        <v>130</v>
-      </c>
-      <c r="B7">
-        <v>1</v>
-      </c>
-      <c r="C7">
-        <v>1</v>
-      </c>
-      <c r="D7">
-        <v>1</v>
-      </c>
-      <c r="E7">
-        <v>1</v>
-      </c>
-      <c r="F7">
-        <v>1.27</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A8">
-        <v>132</v>
-      </c>
-      <c r="B8">
-        <v>1</v>
-      </c>
-      <c r="C8">
-        <v>1</v>
-      </c>
-      <c r="D8">
-        <v>1</v>
-      </c>
-      <c r="E8">
-        <v>1</v>
-      </c>
-      <c r="F8">
-        <v>1.2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A9">
-        <v>170</v>
-      </c>
-      <c r="B9">
-        <v>1</v>
-      </c>
-      <c r="C9">
-        <v>1</v>
-      </c>
-      <c r="D9">
-        <v>1</v>
-      </c>
-      <c r="E9">
-        <v>1</v>
-      </c>
-      <c r="F9">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A10">
-        <v>230</v>
-      </c>
-      <c r="B10">
-        <v>1</v>
-      </c>
-      <c r="C10">
-        <v>1</v>
-      </c>
-      <c r="D10">
-        <v>1</v>
-      </c>
-      <c r="E10">
-        <v>1</v>
-      </c>
-      <c r="F10">
-        <v>1.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>